<commit_message>
aula de ccs parte 2
</commit_message>
<xml_diff>
--- a/CSS/Propriedades.xlsx
+++ b/CSS/Propriedades.xlsx
@@ -4,24 +4,29 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="692"/>
   </bookViews>
   <sheets>
-    <sheet name="fonte" sheetId="1" r:id="rId1"/>
-    <sheet name="texto" sheetId="2" r:id="rId2"/>
-    <sheet name="cor" sheetId="3" r:id="rId3"/>
-    <sheet name="tamanho" sheetId="4" r:id="rId4"/>
-    <sheet name="fundo" sheetId="5" r:id="rId5"/>
-    <sheet name="margem" sheetId="6" r:id="rId6"/>
-    <sheet name="margem-atributo" sheetId="7" r:id="rId7"/>
-    <sheet name="largura-altura" sheetId="8" r:id="rId8"/>
+    <sheet name="seletor" sheetId="13" r:id="rId1"/>
+    <sheet name="fonte" sheetId="1" r:id="rId2"/>
+    <sheet name="texto" sheetId="2" r:id="rId3"/>
+    <sheet name="cor" sheetId="3" r:id="rId4"/>
+    <sheet name="tamanho" sheetId="4" r:id="rId5"/>
+    <sheet name="fundo" sheetId="5" r:id="rId6"/>
+    <sheet name="margem-desenho" sheetId="6" r:id="rId7"/>
+    <sheet name="margem" sheetId="7" r:id="rId8"/>
+    <sheet name="largura-altura" sheetId="8" r:id="rId9"/>
+    <sheet name="display" sheetId="9" r:id="rId10"/>
+    <sheet name="visibility" sheetId="10" r:id="rId11"/>
+    <sheet name="transform" sheetId="11" r:id="rId12"/>
+    <sheet name="pseudo" sheetId="12" r:id="rId13"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="261">
   <si>
     <t>Propriedade</t>
   </si>
@@ -465,6 +470,345 @@
   </si>
   <si>
     <t>altura / largura maxima permitida</t>
+  </si>
+  <si>
+    <t>Propriedades Display</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elemento em nivel de linha </t>
+  </si>
+  <si>
+    <t xml:space="preserve">width e height podem não ter efeito </t>
+  </si>
+  <si>
+    <t>block</t>
+  </si>
+  <si>
+    <t>exibido com obloco (div)</t>
+  </si>
+  <si>
+    <t>acupa por padrão toda largura disponivel</t>
+  </si>
+  <si>
+    <t>inline-block</t>
+  </si>
+  <si>
+    <t>exibição em linha, mas com width e heigth</t>
+  </si>
+  <si>
+    <t>margins e paddings superiores e inferiores podem não ser respeitados</t>
+  </si>
+  <si>
+    <t>margens e paddings superioes e inferiores respeitados</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>oculta o elemento, removendo-o do layout</t>
+  </si>
+  <si>
+    <t>flex, grid, inline-flex, inline-grid.</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Box-shadow</t>
+  </si>
+  <si>
+    <t>valores numericos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">definem a margem, distância com o bloco </t>
+  </si>
+  <si>
+    <t>cor</t>
+  </si>
+  <si>
+    <t>define a cor da sombra</t>
+  </si>
+  <si>
+    <t>Propriedades Visibility</t>
+  </si>
+  <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>elemento visivel</t>
+  </si>
+  <si>
+    <t>hidden</t>
+  </si>
+  <si>
+    <t>elemento ocultado, mas ainda ocupa espaço do layout</t>
+  </si>
+  <si>
+    <t>collapse</t>
+  </si>
+  <si>
+    <t>ocultar linhas e colunas sem alterar o tamanho das mesmas</t>
+  </si>
+  <si>
+    <t>Propriedades Float</t>
+  </si>
+  <si>
+    <t>elemento flutua do lado esquerdo do container</t>
+  </si>
+  <si>
+    <t>elemento flutua do lado direito do container</t>
+  </si>
+  <si>
+    <t>elemento não flutua</t>
+  </si>
+  <si>
+    <t>Propriedades Overflow</t>
+  </si>
+  <si>
+    <t>mesmo fora da região o conteudo sera apresentado</t>
+  </si>
+  <si>
+    <t>elemento cortado quando extrapola a sua área</t>
+  </si>
+  <si>
+    <t>scroll</t>
+  </si>
+  <si>
+    <t>navegador colocará barras de rolagem, com ou sem estrapolação</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>navegador colocará barras de rolagem somente com estrapolação</t>
+  </si>
+  <si>
+    <t>Propriedades Position</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>sticky</t>
+  </si>
+  <si>
+    <t>o único que não "está posicionado"</t>
+  </si>
+  <si>
+    <t>segue o fluxo normal do documento</t>
+  </si>
+  <si>
+    <t>primeiro posicionado de acordo com o documento, depois é delocado com top, left, right, bottom.</t>
+  </si>
+  <si>
+    <t>não afeta os elementos ao redor</t>
+  </si>
+  <si>
+    <t>elemento removido do fluxo normal</t>
+  </si>
+  <si>
+    <t>posicionado de acordo com o ancestral mais proximo posicionado</t>
+  </si>
+  <si>
+    <t>posicionado com relação à viewport (janela do navegador)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posição não se altera com a rolagem da tela </t>
+  </si>
+  <si>
+    <t>se a pagina é impressa, ele aparece na mesma posição em todas as paginas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">posicionado de acordo com o fluxo normal do arquivo </t>
+  </si>
+  <si>
+    <t>ocupa espaço no layout</t>
+  </si>
+  <si>
+    <t>"gruda" no primeiro ancestral com mecanismo de rolagem</t>
+  </si>
+  <si>
+    <t>Propriedades Transform</t>
+  </si>
+  <si>
+    <t>move o elemento da horizontal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">move o elemento da vertical </t>
+  </si>
+  <si>
+    <t>move na vertical e horizontal</t>
+  </si>
+  <si>
+    <t>rotaciona o elemento</t>
+  </si>
+  <si>
+    <t>translateX (50px)</t>
+  </si>
+  <si>
+    <t>translateY (50px)</t>
+  </si>
+  <si>
+    <t>translate (30px, 100px)</t>
+  </si>
+  <si>
+    <t>rotate (45deg)</t>
+  </si>
+  <si>
+    <t>scale (2)</t>
+  </si>
+  <si>
+    <t>escalona o elemento</t>
+  </si>
+  <si>
+    <t>Pseudo Classes</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>estilo inicial do link</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>elemento interage com o usuário</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>estado ativo (botão prescionado)</t>
+  </si>
+  <si>
+    <t>valid / invalid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">campo com valor valido / invalido </t>
+  </si>
+  <si>
+    <t>checked</t>
+  </si>
+  <si>
+    <t>para elementos selecionaveis</t>
+  </si>
+  <si>
+    <t>focus</t>
+  </si>
+  <si>
+    <t>quando o elemento recebe o foco</t>
+  </si>
+  <si>
+    <t>first-child</t>
+  </si>
+  <si>
+    <t>primeiro filho do elemento pai</t>
+  </si>
+  <si>
+    <t>last-child</t>
+  </si>
+  <si>
+    <t>ultimo filho do elemento pai</t>
+  </si>
+  <si>
+    <t>Pseudo Elemento</t>
+  </si>
+  <si>
+    <t>fist-line</t>
+  </si>
+  <si>
+    <t>primeira linha dos paragrafos</t>
+  </si>
+  <si>
+    <t>selected</t>
+  </si>
+  <si>
+    <t>aplicada ao texto que for selecionados</t>
+  </si>
+  <si>
+    <t>after</t>
+  </si>
+  <si>
+    <t>após o conteudo normal</t>
+  </si>
+  <si>
+    <t>before</t>
+  </si>
+  <si>
+    <t>antes do conteudo normal</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>texto do placeholder do form</t>
+  </si>
+  <si>
+    <t>não pode ser utilizados em elemento sem conteudo</t>
+  </si>
+  <si>
+    <t>filho</t>
+  </si>
+  <si>
+    <t>Seletores</t>
+  </si>
+  <si>
+    <t>x &gt; y</t>
+  </si>
+  <si>
+    <t>Sintaxe</t>
+  </si>
+  <si>
+    <t>descendente</t>
+  </si>
+  <si>
+    <t>todo elemento y filho de x, imediatamente descendente</t>
+  </si>
+  <si>
+    <t>todo elemento y descendente de x, filho, neto, bisneto, etc.</t>
+  </si>
+  <si>
+    <t>x  y</t>
+  </si>
+  <si>
+    <t>irmão adjacente</t>
+  </si>
+  <si>
+    <t>x + y</t>
+  </si>
+  <si>
+    <t>primeiro elemento y após x, com mesma descendencia</t>
+  </si>
+  <si>
+    <t>irmão geral</t>
+  </si>
+  <si>
+    <t>x ~ y</t>
+  </si>
+  <si>
+    <t>todo elemento y após x, com mesma descendencia</t>
+  </si>
+  <si>
+    <t>atributo</t>
+  </si>
+  <si>
+    <t>x[atri]</t>
+  </si>
+  <si>
+    <t>todo elemento x com o atributo indicado</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -964,48 +1308,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1015,48 +1332,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1068,9 +1367,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1078,16 +1374,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1114,39 +1401,129 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1442,146 +1819,819 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="77" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30">
+      <c r="A4" s="94" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30">
+      <c r="A5" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="A6" s="94" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>256</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="94" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="D1" s="77" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="77"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30">
+      <c r="A3" s="69" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E3" s="87" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="69"/>
+      <c r="B4" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="87" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30">
+      <c r="A5" s="69"/>
+      <c r="B5" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="87" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30">
+      <c r="A6" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="E6" s="87" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="69"/>
+      <c r="B7" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="A8" s="69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>186</v>
+      </c>
+      <c r="E8" s="77"/>
+    </row>
+    <row r="9" spans="1:5" ht="30">
+      <c r="A9" s="69"/>
+      <c r="B9" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="93" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="59" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="93"/>
+      <c r="E11" s="59" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="83"/>
+      <c r="B12" s="82"/>
+      <c r="D12" s="93" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="77" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="77"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="59" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="93" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="93"/>
+      <c r="E15" s="59" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="93" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="59" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="93"/>
+      <c r="E17" s="59" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="D18" s="93"/>
+      <c r="E18" s="59" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30">
+      <c r="D19" s="93"/>
+      <c r="E19" s="59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30">
+      <c r="D20" s="93" t="s">
+        <v>191</v>
+      </c>
+      <c r="E20" s="59" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="D21" s="93"/>
+      <c r="E21" s="59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30">
+      <c r="D22" s="93"/>
+      <c r="E22" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D10:D11"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75">
+      <c r="A1" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="77"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30">
+      <c r="A5" s="58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75">
+      <c r="A1" s="77" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" s="77"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75">
+      <c r="A1" s="77" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="77"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="27" t="s">
+        <v>230</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75">
+      <c r="A12" s="77" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="77"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.75">
+      <c r="A13" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="94" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="94" t="s">
+        <v>235</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="93" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30">
+      <c r="A17" s="93"/>
+      <c r="B17" s="59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="93" t="s">
+        <v>239</v>
+      </c>
+      <c r="B18" s="59" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30">
+      <c r="A19" s="93"/>
+      <c r="B19" s="59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="94" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20" s="59" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
-      <c r="A11" s="39"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="60"/>
+      <c r="B11" s="24" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40" t="s">
+      <c r="A12" s="60"/>
+      <c r="B12" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40" t="s">
+      <c r="A13" s="60"/>
+      <c r="B13" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40" t="s">
+      <c r="A14" s="60"/>
+      <c r="B14" s="24" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1595,12 +2645,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1613,75 +2663,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="89" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="9" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1694,12 +2744,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1711,139 +2761,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="64" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="62"/>
+      <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="23"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="22" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="65"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="24" t="s">
+      <c r="A7" s="63"/>
+      <c r="B7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="66"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="63"/>
+      <c r="B11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="16" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="22" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="17" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="62"/>
+      <c r="B14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="17" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="24" t="s">
+      <c r="A15" s="63"/>
+      <c r="B15" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1861,7 +2911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1878,78 +2928,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="31" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="69"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="15"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="15"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="69"/>
+      <c r="B7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1964,12 +3014,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1978,84 +3028,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="90" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="55" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="10" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="10" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="10" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E7" s="42"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="10" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="1"/>
@@ -2069,281 +3119,113 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:H15"/>
+  <dimension ref="B4:I15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="1.140625" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="1.5703125" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="1.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="1.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:8">
-      <c r="E4" s="44" t="s">
+    <row r="4" spans="2:9">
+      <c r="F4" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-    </row>
-    <row r="5" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:8" ht="3.75" customHeight="1" thickBot="1">
-      <c r="A6" s="56"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="57"/>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" customHeight="1">
-      <c r="A7" s="56"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="46" t="s">
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+    </row>
+    <row r="5" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="2:9" ht="3.75" customHeight="1" thickBot="1">
+      <c r="B6" s="37"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="38"/>
+    </row>
+    <row r="7" spans="2:9" ht="17.25" customHeight="1">
+      <c r="B7" s="37"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="72" t="s">
+      <c r="F7" s="74"/>
+      <c r="G7" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="G7" s="73"/>
-    </row>
-    <row r="8" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A8" s="56"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="61" t="s">
+      <c r="H7" s="76"/>
+    </row>
+    <row r="8" spans="2:9" ht="27.75" customHeight="1">
+      <c r="B8" s="37"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="57"/>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A9" s="56"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="57"/>
-    </row>
-    <row r="10" spans="1:8" ht="3.75" customHeight="1">
-      <c r="A10" s="56"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="57"/>
-    </row>
-    <row r="11" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A11" s="58"/>
-      <c r="B11" s="74" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="2:9" ht="17.25" customHeight="1" thickBot="1">
+      <c r="B9" s="37"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="38"/>
+    </row>
+    <row r="10" spans="2:9" ht="3.75" customHeight="1">
+      <c r="B10" s="37"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="38"/>
+    </row>
+    <row r="11" spans="2:9" ht="21.75" customHeight="1">
+      <c r="B11" s="39"/>
+      <c r="C11" s="71" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="H15" s="41"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="I15" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-  </mergeCells>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1">
-      <c r="D1" s="76" t="s">
-        <v>129</v>
-      </c>
-      <c r="E1" s="76"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="D2" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="77" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="78" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="79" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="43" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="80" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="80" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="75" t="s">
-        <v>120</v>
-      </c>
-      <c r="D8" s="80" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="75" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="80" t="s">
-        <v>125</v>
-      </c>
-      <c r="B9" s="75" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" s="75" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="80" t="s">
-        <v>126</v>
-      </c>
-      <c r="B10" s="75" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="75" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="75" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2352,9 +3234,215 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75">
+      <c r="A1" s="91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="92"/>
+      <c r="D1" s="77" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="77"/>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1">
+      <c r="A2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="78" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="78" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="91" t="s">
+        <v>163</v>
+      </c>
+      <c r="B12" s="92"/>
+      <c r="D12" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="84" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="87" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B15" s="87" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2366,54 +3454,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="81"/>
+      <c r="B1" s="80"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="55" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="58" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="70" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="31"/>
+      <c r="B5" s="70"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="81" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="83"/>
+      <c r="B7" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
alterando trabalho1 para ex4
</commit_message>
<xml_diff>
--- a/CSS/Propriedades.xlsx
+++ b/CSS/Propriedades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="692"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="692" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="seletor" sheetId="13" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="262">
   <si>
     <t>Propriedade</t>
   </si>
@@ -809,6 +809,9 @@
   </si>
   <si>
     <t>todo elemento x com o atributo indicado</t>
+  </si>
+  <si>
+    <t>horizontal, vertical, blur, cor</t>
   </si>
 </sst>
 </file>
@@ -1420,9 +1423,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,7 +1507,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1485,42 +1524,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1821,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1833,11 +1836,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="54" t="s">
@@ -1851,10 +1854,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="68" t="s">
         <v>244</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="68" t="s">
         <v>246</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -1862,10 +1865,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="68" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="68" t="s">
         <v>251</v>
       </c>
       <c r="C4" s="59" t="s">
@@ -1873,10 +1876,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="68" t="s">
         <v>252</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="68" t="s">
         <v>253</v>
       </c>
       <c r="C5" s="59" t="s">
@@ -1884,10 +1887,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="30">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="68" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="68" t="s">
         <v>256</v>
       </c>
       <c r="C6" s="59" t="s">
@@ -1895,10 +1898,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="68" t="s">
         <v>258</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C7" s="59" t="s">
@@ -1918,7 +1921,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1931,14 +1934,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="D1" s="77" t="s">
+      <c r="B1" s="69"/>
+      <c r="D1" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="E1" s="77"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="54" t="s">
@@ -1954,8 +1957,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="69" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="80" t="s">
         <v>149</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -1964,36 +1967,36 @@
       <c r="D3" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="65" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="69"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="19" t="s">
         <v>151</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="65" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="69"/>
+      <c r="A5" s="80"/>
       <c r="B5" s="19" t="s">
         <v>157</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="65" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="80" t="s">
         <v>152</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -2002,30 +2005,30 @@
       <c r="D6" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="E6" s="87" t="s">
+      <c r="E6" s="65" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="69"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="19" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="80" t="s">
         <v>155</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="69"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="69"/>
+      <c r="A9" s="80"/>
       <c r="B9" s="19" t="s">
         <v>158</v>
       </c>
@@ -2043,7 +2046,7 @@
       <c r="B10" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="94" t="s">
         <v>187</v>
       </c>
       <c r="E10" s="59" t="s">
@@ -2051,21 +2054,21 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="85" t="s">
+      <c r="A11" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="64" t="s">
         <v>161</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="94"/>
       <c r="E11" s="59" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="83"/>
-      <c r="B12" s="82"/>
-      <c r="D12" s="93" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="60"/>
+      <c r="D12" s="94" t="s">
         <v>188</v>
       </c>
       <c r="E12" s="59" t="s">
@@ -2073,11 +2076,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="77"/>
-      <c r="D13" s="93"/>
+      <c r="B13" s="69"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="59" t="s">
         <v>195</v>
       </c>
@@ -2089,7 +2092,7 @@
       <c r="B14" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="94" t="s">
         <v>189</v>
       </c>
       <c r="E14" s="59" t="s">
@@ -2103,7 +2106,7 @@
       <c r="B15" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="D15" s="93"/>
+      <c r="D15" s="94"/>
       <c r="E15" s="59" t="s">
         <v>197</v>
       </c>
@@ -2115,7 +2118,7 @@
       <c r="B16" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="94" t="s">
         <v>190</v>
       </c>
       <c r="E16" s="59" t="s">
@@ -2129,25 +2132,25 @@
       <c r="B17" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="D17" s="93"/>
+      <c r="D17" s="94"/>
       <c r="E17" s="59" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="D18" s="93"/>
+      <c r="D18" s="94"/>
       <c r="E18" s="59" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
-      <c r="D19" s="93"/>
+      <c r="D19" s="94"/>
       <c r="E19" s="59" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30">
-      <c r="D20" s="93" t="s">
+      <c r="D20" s="94" t="s">
         <v>191</v>
       </c>
       <c r="E20" s="59" t="s">
@@ -2155,13 +2158,13 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="D21" s="93"/>
+      <c r="D21" s="94"/>
       <c r="E21" s="59" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30">
-      <c r="D22" s="93"/>
+      <c r="D22" s="94"/>
       <c r="E22" s="59" t="s">
         <v>203</v>
       </c>
@@ -2200,10 +2203,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="54" t="s">
@@ -2260,10 +2263,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="54" t="s">
@@ -2336,10 +2339,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="77"/>
+      <c r="B1" s="69"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="54" t="s">
@@ -2414,10 +2417,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="69" t="s">
         <v>232</v>
       </c>
-      <c r="B12" s="77"/>
+      <c r="B12" s="69"/>
     </row>
     <row r="13" spans="1:2" ht="15.75">
       <c r="A13" s="54" t="s">
@@ -2428,7 +2431,7 @@
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="94" t="s">
+      <c r="A14" s="68" t="s">
         <v>233</v>
       </c>
       <c r="B14" s="59" t="s">
@@ -2436,7 +2439,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="68" t="s">
         <v>235</v>
       </c>
       <c r="B15" s="59" t="s">
@@ -2444,7 +2447,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="94" t="s">
         <v>237</v>
       </c>
       <c r="B16" s="59" t="s">
@@ -2452,13 +2455,13 @@
       </c>
     </row>
     <row r="17" spans="1:2" ht="30">
-      <c r="A17" s="93"/>
+      <c r="A17" s="94"/>
       <c r="B17" s="59" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="93" t="s">
+      <c r="A18" s="94" t="s">
         <v>239</v>
       </c>
       <c r="B18" s="59" t="s">
@@ -2466,13 +2469,13 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="30">
-      <c r="A19" s="93"/>
+      <c r="A19" s="94"/>
       <c r="B19" s="59" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="68" t="s">
         <v>241</v>
       </c>
       <c r="B20" s="59" t="s">
@@ -2498,7 +2501,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2509,11 +2512,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="55" t="s">
@@ -2604,7 +2607,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="70" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="24" t="s">
@@ -2612,25 +2615,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30">
-      <c r="A11" s="60"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="24" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30">
-      <c r="A12" s="60"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30">
-      <c r="A13" s="60"/>
+      <c r="A13" s="70"/>
       <c r="B13" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="60"/>
+      <c r="A14" s="70"/>
       <c r="B14" s="24" t="s">
         <v>88</v>
       </c>
@@ -2650,7 +2653,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2663,20 +2666,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="66" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2749,7 +2752,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2761,11 +2764,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
     </row>
     <row r="2" spans="1:3" ht="15.75">
       <c r="A2" s="55" t="s">
@@ -2779,45 +2782,45 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="79"/>
       <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="72" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="75" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="62"/>
+      <c r="A5" s="73"/>
       <c r="B5" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="65"/>
+      <c r="C5" s="76"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="62"/>
+      <c r="A6" s="73"/>
       <c r="B6" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="65"/>
+      <c r="C6" s="76"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="63"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="66"/>
+      <c r="C7" s="77"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
@@ -2831,7 +2834,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="72" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -2842,7 +2845,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="62"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="9" t="s">
         <v>48</v>
       </c>
@@ -2851,7 +2854,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="63"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="9" t="s">
         <v>49</v>
       </c>
@@ -2860,7 +2863,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="72" t="s">
         <v>66</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -2871,7 +2874,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="62"/>
+      <c r="A13" s="73"/>
       <c r="B13" s="12" t="s">
         <v>52</v>
       </c>
@@ -2880,7 +2883,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="73"/>
       <c r="B14" s="12" t="s">
         <v>53</v>
       </c>
@@ -2889,7 +2892,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="63"/>
+      <c r="A15" s="74"/>
       <c r="B15" s="13" t="s">
         <v>54</v>
       </c>
@@ -2928,18 +2931,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
     </row>
     <row r="2" spans="1:4" ht="15.75">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="77"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="55" t="s">
         <v>72</v>
       </c>
@@ -2948,11 +2951,11 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="81" t="s">
         <v>70</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2960,15 +2963,15 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30">
-      <c r="A4" s="69"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="A4" s="80"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="81"/>
       <c r="D4" s="9" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="80" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2982,7 +2985,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45">
-      <c r="A6" s="69"/>
+      <c r="A6" s="80"/>
       <c r="B6" s="10" t="s">
         <v>78</v>
       </c>
@@ -2992,7 +2995,7 @@
       <c r="D6" s="22"/>
     </row>
     <row r="7" spans="1:4" ht="30">
-      <c r="A7" s="69"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="10" t="s">
         <v>80</v>
       </c>
@@ -3028,14 +3031,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="67" t="s">
         <v>56</v>
       </c>
       <c r="B2" s="55" t="s">
@@ -3140,11 +3143,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:9">
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
     </row>
     <row r="5" spans="2:9" ht="21.75" customHeight="1">
       <c r="B5" s="34"/>
@@ -3168,14 +3171,14 @@
       <c r="B7" s="37"/>
       <c r="C7" s="46"/>
       <c r="D7" s="28"/>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="74"/>
-      <c r="G7" s="75" t="s">
+      <c r="F7" s="85"/>
+      <c r="G7" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="H7" s="76"/>
+      <c r="H7" s="87"/>
     </row>
     <row r="8" spans="2:9" ht="27.75" customHeight="1">
       <c r="B8" s="37"/>
@@ -3208,11 +3211,11 @@
     </row>
     <row r="11" spans="2:9" ht="21.75" customHeight="1">
       <c r="B11" s="39"/>
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
       <c r="F11" s="40"/>
       <c r="G11" s="40"/>
       <c r="H11" s="41"/>
@@ -3234,10 +3237,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3250,14 +3253,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="D1" s="77" t="s">
+      <c r="B1" s="89"/>
+      <c r="D1" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="77"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
       <c r="A2" s="54" t="s">
@@ -3294,10 +3297,10 @@
       <c r="B4" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="90" t="s">
         <v>133</v>
       </c>
     </row>
@@ -3308,8 +3311,8 @@
       <c r="B5" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="91"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="56" t="s">
@@ -3390,10 +3393,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="88" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="92"/>
+      <c r="B12" s="89"/>
       <c r="D12" s="6" t="s">
         <v>137</v>
       </c>
@@ -3410,19 +3413,24 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="62" t="s">
         <v>164</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="65" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="62" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="87" t="s">
+      <c r="B15" s="65" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -3454,10 +3462,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="39" customHeight="1">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="92" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="92"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="55" t="s">
@@ -3479,7 +3487,7 @@
       <c r="A4" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="81" t="s">
         <v>144</v>
       </c>
     </row>
@@ -3487,13 +3495,13 @@
       <c r="A5" s="58" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="70"/>
+      <c r="B5" s="81"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="81" t="s">
+      <c r="B6" s="93" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3501,7 +3509,7 @@
       <c r="A7" s="58" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="81"/>
+      <c r="B7" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>